<commit_message>
exclui figuras de apoio que não entrarão no documento
</commit_message>
<xml_diff>
--- a/data/cinema_results_r.xlsx
+++ b/data/cinema_results_r.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_E9063CDF8F79A8D366075C52F37BD2728A4C7318" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{483FBE53-5DB1-4325-BDE8-497013FD0A3F}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_E9063CDF8F79A8D366075C52F37BD2728A4C7318" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9B3F980-651E-4155-BEB0-40F52B446E08}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,197 +262,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -789,7 +599,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,11 +859,11 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -1081,11 +891,11 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" t="s">
-        <v>15</v>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>

</xml_diff>